<commit_message>
SBP log generator log cleanup fix
</commit_message>
<xml_diff>
--- a/Exes/SBPTestLogGenerator/Assets/DomainConf/SBPClusterTest.xlsx
+++ b/Exes/SBPTestLogGenerator/Assets/DomainConf/SBPClusterTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>Phase</t>
   </si>
@@ -186,12 +186,6 @@
     <t>1-dep on f0t8</t>
   </si>
   <si>
-    <t>1-Incompatible with f0t8</t>
-  </si>
-  <si>
-    <t>f0t1-f0t6</t>
-  </si>
-  <si>
     <t>hint-t1</t>
   </si>
   <si>
@@ -202,6 +196,54 @@
   </si>
   <si>
     <t>hint-t7</t>
+  </si>
+  <si>
+    <t>1-Incompatible with f0t7</t>
+  </si>
+  <si>
+    <t>f0t11</t>
+  </si>
+  <si>
+    <t>t11</t>
+  </si>
+  <si>
+    <t>f0t1-f0t6-f0t11</t>
+  </si>
+  <si>
+    <t>f0t12</t>
+  </si>
+  <si>
+    <t>f0t13</t>
+  </si>
+  <si>
+    <t>f0t14</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>t13</t>
+  </si>
+  <si>
+    <t>t14</t>
+  </si>
+  <si>
+    <t>hint-t12</t>
+  </si>
+  <si>
+    <t>hint-t13</t>
+  </si>
+  <si>
+    <t>f0t15</t>
+  </si>
+  <si>
+    <t>t15</t>
+  </si>
+  <si>
+    <t>hint-t15</t>
+  </si>
+  <si>
+    <t>f0t14-f0t11</t>
   </si>
 </sst>
 </file>
@@ -255,13 +297,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3366FF"/>
+        <fgColor rgb="FFFD898C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,14 +334,14 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -351,8 +393,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,11 +411,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -378,8 +424,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -405,6 +452,8 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -430,6 +479,8 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,13 +810,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -774,7 +825,7 @@
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
@@ -865,59 +916,59 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="9" customFormat="1">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9" t="s">
+    <row r="2" spans="1:25" s="6" customFormat="1" ht="16" thickBot="1">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="R2" s="9">
-        <v>1</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" s="6" customFormat="1">
-      <c r="A3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="F2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="R2" s="6">
+        <v>1</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="8" customFormat="1" ht="16" thickTop="1">
+      <c r="A3" s="8">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="R3" s="6">
-        <v>1</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="6">
+      <c r="G3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="8">
+        <v>1</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="8">
         <v>1</v>
       </c>
     </row>
@@ -938,7 +989,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -952,124 +1003,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="15" customFormat="1">
-      <c r="A5" s="15">
-        <v>0</v>
-      </c>
-      <c r="C5" s="15" t="s">
+    <row r="5" spans="1:25" s="11" customFormat="1">
+      <c r="A5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="R5" s="15">
-        <v>1</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="V5" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" s="11" customFormat="1">
-      <c r="A6" s="11">
-        <v>0</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+      <c r="R5" s="11">
+        <v>1</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="15" customFormat="1">
+      <c r="A6" s="15">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="11">
-        <v>1</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V6" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" s="11" customFormat="1">
-      <c r="A7" s="11">
-        <v>0</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="R6" s="15">
+        <v>1</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V6" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="15" customFormat="1" ht="16" thickBot="1">
+      <c r="A7" s="15">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="11" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="11">
-        <v>1</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V7" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" s="6" customFormat="1">
-      <c r="A8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="R7" s="15">
+        <v>1</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V7" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" s="8" customFormat="1" ht="16" thickTop="1">
+      <c r="A8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="R8" s="6">
-        <v>1</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V8" s="6">
+      <c r="G8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="R8" s="8">
+        <v>1</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V8" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1090,125 +1141,250 @@
         <v>47</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
+        <v>31</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" s="11" customFormat="1">
+      <c r="A10" s="11">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="R10" s="11">
+        <v>1</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="15" customFormat="1">
+      <c r="A11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="H11" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="R11" s="15">
+        <v>1</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V11" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" s="19" customFormat="1" ht="16" thickBot="1">
+      <c r="A12" s="19">
+        <v>0</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="K12" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="R12" s="19">
+        <v>1</v>
+      </c>
+      <c r="U12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="V12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" s="8" customFormat="1" ht="16" thickTop="1">
+      <c r="A13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="U9" t="s">
-        <v>31</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" s="15" customFormat="1">
-      <c r="A10" s="15">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="D13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>31</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="U16" t="s">
+        <v>31</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="11" customFormat="1">
+      <c r="A17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="R10" s="15">
-        <v>1</v>
-      </c>
-      <c r="U10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="V10" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" s="11" customFormat="1">
-      <c r="A11" s="11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="H11" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="R11" s="11">
-        <v>1</v>
-      </c>
-      <c r="U11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V11" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" s="11" customFormat="1">
-      <c r="A12" s="11">
-        <v>0</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="K12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="R12" s="11">
-        <v>1</v>
-      </c>
-      <c r="U12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V12" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:25">
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="6:6">
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="6:6">
+      <c r="F17" s="12"/>
+      <c r="R17" s="11">
+        <v>1</v>
+      </c>
+      <c r="U17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V17" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="1:22">
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="1:22">
       <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="F21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>